<commit_message>
classes 4 and 5
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -28,13 +28,13 @@
     <t>Problem-solving searching review</t>
   </si>
   <si>
-    <t>Adversarial search and games review</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning Tooling and Environments</t>
+    <t>Problem-solving, Adversarial search and games review</t>
   </si>
   <si>
     <t>Q-Learning Algorithm</t>
+  </si>
+  <si>
+    <t>Q-Learning Algorithm, Reinforcement Learning Tooling and Environments</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,12 +104,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -147,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -158,13 +152,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -172,9 +163,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,9 +472,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="65.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="70.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -496,7 +484,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="2">
@@ -517,7 +505,7 @@
       <c r="C3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>44971</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -526,25 +514,25 @@
       <c r="C4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>44973</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A6" s="4">
+        <v>44980</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A6" s="5">
-        <v>44980</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="63.75" customFormat="1" s="1">
-      <c r="A7" s="5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A7" s="4">
         <v>44985</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -554,8 +542,8 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="63.75" customFormat="1" s="1">
-      <c r="A8" s="5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A8" s="4">
         <v>44987</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -563,8 +551,8 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="63.75" customFormat="1" s="1">
-      <c r="A9" s="5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A9" s="4">
         <v>44992</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -572,8 +560,8 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="53.25" customFormat="1" s="1">
-      <c r="A10" s="5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A10" s="4">
         <v>44994</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -581,8 +569,8 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="53.25" customFormat="1" s="1">
-      <c r="A11" s="5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A11" s="4">
         <v>44999</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -590,8 +578,8 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A12" s="5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A12" s="4">
         <v>45001</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -599,8 +587,8 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A13" s="5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A13" s="4">
         <v>45006</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -608,8 +596,8 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A14" s="5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A14" s="4">
         <v>45008</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -618,34 +606,34 @@
       <c r="C14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>45013</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>45015</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>45020</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>45022</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -654,7 +642,7 @@
       <c r="C18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="41.25" customFormat="1" s="1">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>45027</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -663,7 +651,7 @@
       <c r="C19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>45029</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -672,7 +660,7 @@
       <c r="C20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>45034</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -681,7 +669,7 @@
       <c r="C21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>45036</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -690,7 +678,7 @@
       <c r="C22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>45041</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -705,10 +693,10 @@
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>45048</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -717,7 +705,7 @@
       <c r="C25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>45050</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -726,7 +714,7 @@
       <c r="C26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>45055</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -735,46 +723,46 @@
       <c r="C27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>45057</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>45062</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>45064</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>45069</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>45071</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="3"/>
@@ -783,10 +771,10 @@
       <c r="A33" s="2">
         <v>45076</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A34" s="2">
@@ -795,7 +783,7 @@
       <c r="B34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A35" s="2">
@@ -804,17 +792,17 @@
       <c r="B35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
+      <c r="C36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="C37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
double deep q-learning project
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Implementing an agent to deal with an environment a little more complex</t>
   </si>
   <si>
-    <t>Deep Neural Networks review</t>
+    <t>Deep Q-Learning</t>
   </si>
   <si>
     <t>Midterm assessment - we do not have classes</t>
@@ -67,13 +67,10 @@
     <t>We do not have classes</t>
   </si>
   <si>
-    <t>Neural Network Policies</t>
-  </si>
-  <si>
-    <t>Deep Q-Learning</t>
-  </si>
-  <si>
-    <t>Double Deep Q-Learning</t>
+    <t>Deep Q-Learning studio</t>
+  </si>
+  <si>
+    <t>Double Deep Q-Learning project</t>
   </si>
   <si>
     <t>Policy Optimization Algorithms (PPO)</t>
@@ -486,7 +483,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A2" s="2">
         <v>44964</v>
       </c>
@@ -495,7 +492,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A3" s="2">
         <v>44966</v>
       </c>
@@ -504,7 +501,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A4" s="4">
         <v>44971</v>
       </c>
@@ -513,7 +510,7 @@
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A5" s="4">
         <v>44973</v>
       </c>
@@ -522,7 +519,7 @@
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A6" s="4">
         <v>44980</v>
       </c>
@@ -605,7 +602,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A15" s="4">
         <v>45013</v>
       </c>
@@ -614,7 +611,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A16" s="4">
         <v>45015</v>
       </c>
@@ -623,7 +620,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="41.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A17" s="4">
         <v>45020</v>
       </c>
@@ -632,7 +629,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="41.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A18" s="4">
         <v>45022</v>
       </c>
@@ -641,7 +638,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="41.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A19" s="4">
         <v>45027</v>
       </c>
@@ -650,16 +647,16 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A20" s="4">
         <v>45029</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A21" s="4">
         <v>45034</v>
       </c>
@@ -668,21 +665,21 @@
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A22" s="4">
         <v>45036</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A23" s="4">
         <v>45041</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -691,7 +688,7 @@
         <v>45043</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3"/>
     </row>
@@ -700,7 +697,7 @@
         <v>45048</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3"/>
     </row>
@@ -709,7 +706,7 @@
         <v>45050</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3"/>
     </row>
@@ -718,7 +715,7 @@
         <v>45055</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3"/>
     </row>
@@ -727,7 +724,7 @@
         <v>45057</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3"/>
     </row>
@@ -736,7 +733,7 @@
         <v>45062</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C29" s="3"/>
     </row>
@@ -745,7 +742,7 @@
         <v>45064</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C30" s="3"/>
     </row>
@@ -754,7 +751,7 @@
         <v>45069</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="3"/>
     </row>
@@ -763,7 +760,7 @@
         <v>45071</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="3"/>
     </row>
@@ -772,7 +769,7 @@
         <v>45076</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="3"/>
     </row>
@@ -781,7 +778,7 @@
         <v>45078</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="3"/>
     </row>
@@ -790,7 +787,7 @@
         <v>45083</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="3"/>
     </row>

</xml_diff>

<commit_message>
plano de aula atualizado
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Data</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Agente Autônomo e Busca em Espaço de Estados</t>
   </si>
   <si>
-    <t xml:space="preserve">Aula expositiva com roteiro de implementação. Entrega da implementação prevista para 18-fev.</t>
+    <t xml:space="preserve">Aula expositiva com roteiro de implementação. </t>
   </si>
   <si>
     <t>12-Fev</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Busca em Espaço de Estados e Teoria de Jogos</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação do problema e implementação da solução em grupo. Entrega da implementação prevista para 21-fev. </t>
+    <t xml:space="preserve">Apresentação do problema e implementação da solução em grupo. </t>
   </si>
   <si>
     <t>21-Fev</t>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">Algoritmo Q-Learning</t>
   </si>
   <si>
+    <t xml:space="preserve">Aula expositiva acom roteiro de implementação. </t>
+  </si>
+  <si>
     <t>28-Fev</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t xml:space="preserve">Revisão: Q-Learning, SARSA, ambientes determinísticos ou não, avaliação de agentes</t>
   </si>
   <si>
+    <t xml:space="preserve">Debate em sala de aula sobre resultados alcançados até então com as implementações realizadas.</t>
+  </si>
+  <si>
     <t>18-Março</t>
   </si>
   <si>
@@ -154,7 +160,7 @@
     <t>10-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Comparando Deep Q-Learning com Reinforce</t>
+    <t xml:space="preserve">Comparando Deep Q-Learning e Reinforce</t>
   </si>
   <si>
     <t>15-Abril</t>
@@ -970,7 +976,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1080,287 +1086,339 @@
       <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" s="3" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="5"/>
+        <v>62</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="36" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A36" s="4"/>
@@ -1403,492 +1461,492 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificacoes pos primeira aula
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Data</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">Algoritmo Q-Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula expositiva acom roteiro de implementação. </t>
   </si>
   <si>
     <t>28-Fev</t>
@@ -383,7 +380,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -392,20 +389,10 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="8.000000"/>
-      <color indexed="64"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -429,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -446,22 +433,19 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
@@ -976,7 +960,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1045,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1053,10 +1037,10 @@
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1065,10 +1049,10 @@
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1077,347 +1061,347 @@
       </c>
     </row>
     <row r="8" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="14" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A23" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A25" s="9" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A26" s="9" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A29" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A29" s="9" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="9" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A31" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="8" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="A32" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>62</v>
+      <c r="B32" s="10"/>
+      <c r="C32" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>62</v>
+      <c r="C33" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1453,500 +1437,500 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="12" width="84.433571428571426"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="11" width="84.433571428571426"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="2" width="52.290714285714287"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="12" width="70.433571428571426"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="12" width="43.719285714285718"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="11" width="70.433571428571426"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="11" width="43.719285714285718"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>105</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="C29" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="C32" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
informando data especifica para a prova
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="175">
   <si>
     <t>Questions</t>
   </si>
@@ -524,6 +524,15 @@
     <t>27-Maio</t>
   </si>
   <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Sem aula</t>
+  </si>
+  <si>
+    <t>29-Maio</t>
+  </si>
+  <si>
     <t>Avaliação final</t>
   </si>
   <si>
@@ -531,9 +540,6 @@
   </si>
   <si>
     <t>Avaliação Final</t>
-  </si>
-  <si>
-    <t>29-Maio</t>
   </si>
 </sst>
 </file>
@@ -541,19 +547,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -595,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -606,25 +606,22 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,671 +932,671 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="27.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="93.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="75.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="145.57642857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="103.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="27.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="93.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="75.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="145.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="103.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="36.75" customFormat="1" s="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="24.75" customFormat="1" s="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="3" t="s">
         <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A30" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A30" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A31" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A31" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A32" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A32" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="3" t="s">
         <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>171</v>
+      <c r="D35" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1617,17 +1614,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="84.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="52.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="70.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="43.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="84.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="52.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="70.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="43.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1638,478 +1635,478 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18" customFormat="1" s="1">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
material para a aula sobre o algoritmo sarsa
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Data</t>
   </si>
@@ -58,6 +58,9 @@
     <t>05-Fev</t>
   </si>
   <si>
+    <t>10-Fev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Algoritmos Tabulares (Q-Learning e Sarsa)</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t xml:space="preserve">Aula expositiva com roteiro de implementação. </t>
   </si>
   <si>
-    <t>10-Fev</t>
+    <t>12-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Como implementar uma solução usando o algoritmo Q-Learning?</t>
@@ -85,7 +88,13 @@
     <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Q-learning e aplicá-lo em diversas situações.</t>
   </si>
   <si>
-    <t>12-Fev</t>
+    <t>17-Fev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem aula</t>
+  </si>
+  <si>
+    <t>19-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Como funciona o algoritmo Sarsa e quais são as diferenças entre o Q-Learning e Sarsa? </t>
@@ -97,7 +106,7 @@
     <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Sarsa</t>
   </si>
   <si>
-    <t>17-Fev</t>
+    <t>24-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">Como avaliar a performance de um agente que usa RL e a sua curva de aprendizado? </t>
@@ -109,7 +118,7 @@
     <t xml:space="preserve">Estudantes são capazes de avaliar o desempenho de uma implementação usando RL</t>
   </si>
   <si>
-    <t>19-Fev</t>
+    <t>26-Fev</t>
   </si>
   <si>
     <t xml:space="preserve">É possível usar RL em ambientes não determinísticos? </t>
@@ -124,7 +133,7 @@
     <t xml:space="preserve">Apresentação do problema e implementação da solução em grupo. </t>
   </si>
   <si>
-    <t>24-Fev</t>
+    <t>10-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Quais são os limites dos algoritmos Q-Learning e Sarsa? </t>
@@ -139,7 +148,7 @@
     <t xml:space="preserve">Debate em sala de aula sobre resultados alcançados até então com as implementações realizadas.</t>
   </si>
   <si>
-    <t>26-Fev</t>
+    <t>12-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Deep Reinforcement Learning: value-based e policy gradient</t>
@@ -151,7 +160,7 @@
     <t xml:space="preserve">Implementando um agente que precisa lidar com um ambiente mais complexo</t>
   </si>
   <si>
-    <t>10-Março</t>
+    <t>17-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Como funciona o algoritmo Deep Q-Learning?</t>
@@ -163,7 +172,7 @@
     <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Deep Q-Learning</t>
   </si>
   <si>
-    <t>12-Março</t>
+    <t>19-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Como implementar o algoritmo Deep Q-Learning? Quais são os detalhes de implementação e como usar?</t>
@@ -175,19 +184,31 @@
     <t xml:space="preserve">Estudantes são capazes de identificar qual a melhor arquitetura de rede neural para um determinado problema</t>
   </si>
   <si>
-    <t>17-Março</t>
-  </si>
-  <si>
-    <t>19-Março</t>
+    <t>24-Março</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variantes do algoritmo Deep Q-Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de implementar variantes do algoritmo Deep Q-Learning</t>
+  </si>
+  <si>
+    <t>26-Março</t>
+  </si>
+  <si>
+    <t>31-Março</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semana de avaliações intermediárias (não teremos aula): implementação do projeto 1</t>
   </si>
   <si>
     <t xml:space="preserve">Implementação do projeto 1</t>
   </si>
   <si>
-    <t>24-Março</t>
-  </si>
-  <si>
-    <t>26-Março</t>
+    <t>02-Abril</t>
+  </si>
+  <si>
+    <t>7-Abril</t>
   </si>
   <si>
     <t xml:space="preserve">Como funciona o algoritmo Reinforce e o conceito de policy gradient?</t>
@@ -199,18 +220,6 @@
     <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Reinforce</t>
   </si>
   <si>
-    <t>31-Março</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semana de avaliações intermediárias - não teremos aula</t>
-  </si>
-  <si>
-    <t>02-Abril</t>
-  </si>
-  <si>
-    <t>7-Abril</t>
-  </si>
-  <si>
     <t>9-Abril</t>
   </si>
   <si>
@@ -271,6 +280,9 @@
     <t>30-Abril</t>
   </si>
   <si>
+    <t xml:space="preserve">Projeto Final</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quais são as principais implementações de DDPG e PPO disponíveis? </t>
   </si>
   <si>
@@ -283,9 +295,6 @@
     <t>5-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Projeto Final</t>
-  </si>
-  <si>
     <t xml:space="preserve">Que tipo de problema pode-se resolver com RL?</t>
   </si>
   <si>
@@ -325,19 +334,13 @@
     <t>21-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Finalização do texto e da apresentação (introdução, objetivos, ambiente, método, resultados e considerações finais)</t>
+    <t xml:space="preserve">Apresentação final do projeto</t>
   </si>
   <si>
     <t>26-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentando o projeto</t>
-  </si>
-  <si>
-    <t>Apresentações</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apresentações dos projetos</t>
+    <t xml:space="preserve">Não teremos aula</t>
   </si>
   <si>
     <t>28-Maio</t>
@@ -512,7 +515,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -521,21 +524,31 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.000000"/>
-      <color indexed="64"/>
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -559,10 +572,11 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -570,42 +584,46 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1114,7 +1132,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1168,274 +1186,274 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" ht="20.25" customHeight="1">
+    <row r="3" s="2" customFormat="1" ht="36.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>38</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" s="2" customFormat="1" ht="24.75" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>54</v>
+      <c r="B14" s="7"/>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="2" t="s">
+    </row>
+    <row r="17" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1444,326 +1462,326 @@
         <v>63</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="6"/>
+        <v>67</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" s="2" customFormat="1" ht="24.75" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="6"/>
+        <v>79</v>
+      </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="7"/>
+        <v>83</v>
+      </c>
+      <c r="B23" s="6"/>
       <c r="C23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="20.25" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="24.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>88</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="7"/>
+        <v>101</v>
+      </c>
+      <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="6"/>
+        <v>102</v>
+      </c>
+      <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="11"/>
+        <v>104</v>
+      </c>
+      <c r="B30" s="12"/>
       <c r="C30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>103</v>
+      <c r="A31" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>107</v>
+      <c r="A32" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A33" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="12"/>
+      <c r="A33" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="C33" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A34" s="13" t="s">
+      <c r="E34" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="36" s="2" customFormat="1" ht="20.25" customHeight="1"/>
     <row r="37" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1794,492 +1812,492 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao do plano de aula
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>Data</t>
   </si>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">Como implementar o algoritmo Deep Q-Learning? Quais são os detalhes de implementação e como usar?</t>
   </si>
   <si>
-    <t xml:space="preserve">Revisão sobre Redes Neurais e decisões de projeto de RN para RL</t>
+    <t xml:space="preserve">Variantes do algoritmo Deep Q-Learning</t>
   </si>
   <si>
     <t xml:space="preserve">Estudantes são capazes de identificar qual a melhor arquitetura de rede neural para um determinado problema</t>
@@ -187,21 +187,30 @@
     <t>24-Março</t>
   </si>
   <si>
-    <t xml:space="preserve">Variantes do algoritmo Deep Q-Learning</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estudantes são capazes de implementar variantes do algoritmo Deep Q-Learning</t>
   </si>
   <si>
     <t>26-Março</t>
   </si>
   <si>
+    <t xml:space="preserve">Como funciona o algoritmo Reinforce e o conceito de policy gradient?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algoritmo Reinforce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Reinforce</t>
+  </si>
+  <si>
     <t>31-Março</t>
   </si>
   <si>
     <t xml:space="preserve">Semana de avaliações intermediárias (não teremos aula): implementação do projeto 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Sem aula: implementação de APSs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implementação do projeto 1</t>
   </si>
   <si>
@@ -211,22 +220,13 @@
     <t>7-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Como funciona o algoritmo Reinforce e o conceito de policy gradient?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algoritmo Reinforce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de implementar o algoritmo Reinforce</t>
+    <t xml:space="preserve">Enunciado do projeto intermediário</t>
   </si>
   <si>
     <t>9-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Quais são as diferenças entre Deep Q-Learning e Reinforce? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparando Deep Q-Learning e Reinforce</t>
+    <t xml:space="preserve">Revisão e discussão sobre os resultados obtidos com as últimas APSs</t>
   </si>
   <si>
     <t xml:space="preserve">Estudantes são capazes de enumerar as diferenças entre os algoritmos Deep Q-Learning e Reinforce</t>
@@ -238,6 +238,18 @@
     <t xml:space="preserve">Deep Reinforcement Learning: actor-critic</t>
   </si>
   <si>
+    <t xml:space="preserve">Como funciona o algoritmo A2C?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actor-Critic (A2C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de entender o funcionamento do algoritmo A2C</t>
+  </si>
+  <si>
+    <t>16-Abril</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como funciona o algoritmo DDPG?</t>
   </si>
   <si>
@@ -247,15 +259,6 @@
     <t xml:space="preserve">Estudantes são capazes de entender o funcionamento do algoritmo DDPG</t>
   </si>
   <si>
-    <t>16-Abril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quais são os detalhes de implementação do algoritmo DDPG?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de utilizar implementações de DDPG para treinar agentes</t>
-  </si>
-  <si>
     <t>23-Abril</t>
   </si>
   <si>
@@ -271,10 +274,10 @@
     <t>28-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Quais são os detalhes de implementação do algoritmo PPO?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de utilizar implementações de PPO para treinar agentes</t>
+    <t xml:space="preserve">Ambientes multi-agent e criação de ambientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de entender a diferente entre single e multi-agent e sabem como implementar os seus próprios ambientes</t>
   </si>
   <si>
     <t>30-Abril</t>
@@ -283,10 +286,7 @@
     <t xml:space="preserve">Projeto Final</t>
   </si>
   <si>
-    <t xml:space="preserve">Quais são as principais implementações de DDPG e PPO disponíveis? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reutilizando implementações de DDPG e PPO em projetos</t>
+    <t xml:space="preserve">RLHF e uso de RL em LLMs</t>
   </si>
   <si>
     <t xml:space="preserve">Estudantes são capazes de escolher as melhores implementações de DDPG e PPO entre bibliotecas disponíveis.</t>
@@ -319,10 +319,13 @@
     <t>12-Maio</t>
   </si>
   <si>
+    <t xml:space="preserve">Apresentação dos resultados do projeto intermediário</t>
+  </si>
+  <si>
+    <t>14-Maio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implementação do projeto</t>
-  </si>
-  <si>
-    <t>14-Maio</t>
   </si>
   <si>
     <t>19-Maio</t>
@@ -602,11 +605,11 @@
     <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1132,7 +1135,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1375,7 +1378,7 @@
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1390,14 +1393,14 @@
         <v>55</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>18</v>
@@ -1405,70 +1408,70 @@
     </row>
     <row r="15" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A16" s="10" t="s">
-        <v>59</v>
+      <c r="A16" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="9" t="s">
-        <v>60</v>
+      <c r="C16" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A17" s="10" t="s">
-        <v>62</v>
+      <c r="A17" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>18</v>
@@ -1476,10 +1479,10 @@
     </row>
     <row r="19" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>69</v>
@@ -1498,13 +1501,13 @@
       <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="10" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1520,10 +1523,10 @@
         <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>18</v>
@@ -1531,16 +1534,16 @@
     </row>
     <row r="22" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>18</v>
@@ -1548,17 +1551,17 @@
     </row>
     <row r="23" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>18</v>
@@ -1566,13 +1569,13 @@
     </row>
     <row r="24" s="2" customFormat="1" ht="24.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>89</v>
@@ -1644,7 +1647,7 @@
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>93</v>
@@ -1658,11 +1661,11 @@
     </row>
     <row r="29" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>93</v>
@@ -1671,95 +1674,95 @@
         <v>94</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A31" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A32" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A33" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A34" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1"/>
@@ -1812,184 +1815,184 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2000,10 +2003,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2014,290 +2017,290 @@
         <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comentarios sobre implementacoes das APSs
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>Data</t>
   </si>
@@ -250,250 +250,247 @@
     <t>16-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Como funciona o algoritmo DDPG?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep Deterministic Policy Gradient (DDPG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de entender o funcionamento do algoritmo DDPG</t>
+    <t xml:space="preserve">Como funciona o algoritmo PPO?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proximal Policy Optimization Algorithms (PPO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de entender o funcionamento do algoritmo PPO</t>
   </si>
   <si>
     <t>23-Abril</t>
   </si>
   <si>
-    <t xml:space="preserve">Como funciona o algoritmo PPO?</t>
+    <t xml:space="preserve">Ambientes multi-agent e criação de ambientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de entender a diferente entre single e multi-agent e sabem como implementar os seus próprios ambientes</t>
+  </si>
+  <si>
+    <t>28-Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula studio </t>
+  </si>
+  <si>
+    <t>30-Abril</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projeto Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RLHF e uso de RL em LLMs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudantes são capazes de escolher as melhores implementações de DDPG e PPO entre bibliotecas disponíveis.</t>
+  </si>
+  <si>
+    <t>5-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Que tipo de problema pode-se resolver com RL?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula Studio para execução do projeto final</t>
+  </si>
+  <si>
+    <t>7-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definindo o escopo do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega do título do projeto e da descrição do ambiente (environment)</t>
+  </si>
+  <si>
+    <t>12-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação dos resultados do projeto intermediário</t>
+  </si>
+  <si>
+    <t>14-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação do projeto</t>
+  </si>
+  <si>
+    <t>19-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega da descrição dos métodos e resultados</t>
+  </si>
+  <si>
+    <t>21-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apresentação final do projeto</t>
+  </si>
+  <si>
+    <t>26-Maio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não teremos aula</t>
+  </si>
+  <si>
+    <t>28-Maio</t>
+  </si>
+  <si>
+    <t>2-Junho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação final</t>
+  </si>
+  <si>
+    <t>Avaliação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação Final</t>
+  </si>
+  <si>
+    <t>4-Junho</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Program/Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is Reinforcement Learning? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Reinforcement Learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to discuss the main concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lectures, use cases and implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the differences between problem-solving searching and RL? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem-solving searching review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement solution for simple problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the differences between adversarial search and RL? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem-solving, Adversarial search and games review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q-Learning algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q-Learning Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement a Q-Learning algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q-Learning Algorithm, Reinforcement Learning Tooling and Environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sarsa algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARSA Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement a Sarsa algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the differences between Q-Learning and Sarsa? How to measure those differences? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to evaluate the performance of an agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students understand how to evaluate a RL solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it possible to use RL in non-deterministic environments? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using RL in non-deterministic environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement solutions for non-deterministic environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it possible to use RL in competitive environments?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using RL in a competitive environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement solutions for competitive environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using RL in a competitive environment with random behavior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I would like to work with problems that are more complex....</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementing an agent to deal with an environment a little more complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement and use Q-Learning algorithm in several situations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to implement a Deep Q-Learning algorithm? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm assessment - we do not have classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to use a Deep Q-Learning algorithm? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We do not have classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep Q-Learning studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement and use Deep Q-Learning algorithm in several situations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to implement a Double Deep Q-Learning? Which are the differences between DDQL and DQL? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Deep Q-Learning project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students are able to implement and use Double Deep Q-Learning algorithm in several situations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is DDQL really works? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policy Optimization Algorithms</t>
   </si>
   <si>
     <t xml:space="preserve">Policy Optimization Algorithms (PPO)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de entender o funcionamento do algoritmo PPO</t>
-  </si>
-  <si>
-    <t>28-Abril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ambientes multi-agent e criação de ambientes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de entender a diferente entre single e multi-agent e sabem como implementar os seus próprios ambientes</t>
-  </si>
-  <si>
-    <t>30-Abril</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projeto Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RLHF e uso de RL em LLMs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudantes são capazes de escolher as melhores implementações de DDPG e PPO entre bibliotecas disponíveis.</t>
-  </si>
-  <si>
-    <t>5-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Que tipo de problema pode-se resolver com RL?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula Studio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento do projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula Studio para execução do projeto final</t>
-  </si>
-  <si>
-    <t>7-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definindo o escopo do projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrega do título do projeto e da descrição do ambiente (environment)</t>
-  </si>
-  <si>
-    <t>12-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apresentação dos resultados do projeto intermediário</t>
-  </si>
-  <si>
-    <t>14-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementação do projeto</t>
-  </si>
-  <si>
-    <t>19-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entrega da descrição dos métodos e resultados</t>
-  </si>
-  <si>
-    <t>21-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apresentação final do projeto</t>
-  </si>
-  <si>
-    <t>26-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Não teremos aula</t>
-  </si>
-  <si>
-    <t>28-Maio</t>
-  </si>
-  <si>
-    <t>2-Junho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação final</t>
-  </si>
-  <si>
-    <t>Avaliação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação Final</t>
-  </si>
-  <si>
-    <t>4-Junho</t>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Evidence</t>
-  </si>
-  <si>
-    <t>Program/Activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is Reinforcement Learning? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Reinforcement Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to discuss the main concepts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lectures, use cases and implementation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are the differences between problem-solving searching and RL? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problem-solving searching review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement solution for simple problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are the differences between adversarial search and RL? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problem-solving, Adversarial search and games review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q-Learning algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q-Learning Algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement a Q-Learning algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q-Learning Algorithm, Reinforcement Learning Tooling and Environments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sarsa algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARSA Algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement a Sarsa algorithm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are the differences between Q-Learning and Sarsa? How to measure those differences? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to evaluate the performance of an agent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students understand how to evaluate a RL solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is it possible to use RL in non-deterministic environments? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using RL in non-deterministic environments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement solutions for non-deterministic environments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is it possible to use RL in competitive environments?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using RL in a competitive environment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement solutions for competitive environments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using RL in a competitive environment with random behavior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I would like to work with problems that are more complex....</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementing an agent to deal with an environment a little more complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement and use Q-Learning algorithm in several situations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to implement a Deep Q-Learning algorithm? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midterm assessment - we do not have classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to use a Deep Q-Learning algorithm? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">We do not have classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep Q-Learning studio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement and use Deep Q-Learning algorithm in several situations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to implement a Double Deep Q-Learning? Which are the differences between DDQL and DQL? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Double Deep Q-Learning project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Students are able to implement and use Double Deep Q-Learning algorithm in several situations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is DDQL really works? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Policy Optimization Algorithms</t>
   </si>
   <si>
     <t xml:space="preserve">Students are able to implement and use PPO in several situations</t>
@@ -1135,7 +1132,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E15" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1453,7 +1450,7 @@
       <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1501,13 +1498,13 @@
       <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="2" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -1540,10 +1537,10 @@
         <v>81</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>18</v>
@@ -1551,37 +1548,37 @@
     </row>
     <row r="23" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>18</v>
+      <c r="D23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="24.75" customHeight="1">
       <c r="A24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="D24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>18</v>
@@ -1589,180 +1586,180 @@
     </row>
     <row r="25" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A31" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A32" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A33" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A34" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1"/>
@@ -1815,184 +1812,184 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2003,10 +2000,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2017,290 +2014,290 @@
         <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizado enunciado projeto final
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Data</t>
   </si>
@@ -283,16 +283,16 @@
     <t xml:space="preserve">Projeto Final</t>
   </si>
   <si>
+    <t xml:space="preserve">Definindo o escopo do projeto final</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aula studio </t>
   </si>
   <si>
     <t>5-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Que tipo de problema pode-se resolver com RL?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aula Studio</t>
+    <t xml:space="preserve">Desenvolvimento dos projetos</t>
   </si>
   <si>
     <t xml:space="preserve">Desenvolvimento do projeto</t>
@@ -304,9 +304,6 @@
     <t>7-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Definindo o escopo do projeto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Entrega do título do projeto e da descrição do ambiente (environment)</t>
   </si>
   <si>
@@ -319,19 +316,19 @@
     <t>14-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementação do projeto</t>
+    <t xml:space="preserve">Apresentação do status do projeto final</t>
   </si>
   <si>
     <t>19-Maio</t>
   </si>
   <si>
+    <t xml:space="preserve">Apresentação final do projeto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entrega da descrição dos métodos e resultados</t>
   </si>
   <si>
     <t>21-Maio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apresentação final do projeto</t>
   </si>
   <si>
     <t>26-Maio</t>
@@ -576,7 +573,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -604,6 +601,9 @@
     </xf>
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1568,28 +1568,28 @@
       <c r="B24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="10" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1605,28 +1605,28 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>92</v>
@@ -1637,14 +1637,14 @@
     </row>
     <row r="28" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>92</v>
@@ -1655,14 +1655,14 @@
     </row>
     <row r="29" s="2" customFormat="1" ht="20.25" customHeight="1">
       <c r="A29" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>91</v>
+      <c r="D29" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>92</v>
@@ -1675,88 +1675,88 @@
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="11"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A31" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A31" s="12" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A32" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A32" s="12" t="s">
+      <c r="B32" s="12"/>
+      <c r="C32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A33" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A33" s="13" t="s">
+      <c r="C33" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A34" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A34" s="13" t="s">
-        <v>112</v>
-      </c>
       <c r="C34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1"/>
@@ -1765,17 +1765,17 @@
       <c r="A37" s="3"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1809,184 +1809,184 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1997,10 +1997,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2011,290 +2011,290 @@
         <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao do material sobre ppo
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>Data</t>
   </si>
@@ -331,6 +331,15 @@
     <t>21-Maio</t>
   </si>
   <si>
+    <t xml:space="preserve">Avaliação final</t>
+  </si>
+  <si>
+    <t>Avaliação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação Final</t>
+  </si>
+  <si>
     <t>26-Maio</t>
   </si>
   <si>
@@ -338,21 +347,6 @@
   </si>
   <si>
     <t>28-Maio</t>
-  </si>
-  <si>
-    <t>2-Junho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação final</t>
-  </si>
-  <si>
-    <t>Avaliação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação Final</t>
-  </si>
-  <si>
-    <t>4-Junho</t>
   </si>
   <si>
     <t>Questions</t>
@@ -573,7 +567,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -602,9 +596,6 @@
     <xf fontId="3" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -612,9 +603,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1568,7 +1556,7 @@
       <c r="B24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1657,7 +1645,7 @@
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="11"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="3" t="s">
         <v>101</v>
       </c>
@@ -1675,110 +1663,88 @@
       <c r="A30" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A31" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="12"/>
+      <c r="A31" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="11"/>
       <c r="C31" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A32" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="12"/>
+      <c r="A32" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="11"/>
       <c r="C32" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A33" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A34" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="36" s="2" customFormat="1" ht="20.25" customHeight="1"/>
+      <c r="A34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" s="2" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
     <row r="37" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" s="2" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1809,184 +1775,184 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="18" customHeight="1">
@@ -1997,10 +1963,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="18" customHeight="1">
@@ -2011,290 +1977,290 @@
         <v>49</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A35" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alteracao na forma de entrega dos projetos
</commit_message>
<xml_diff>
--- a/lessons_plan.xlsx
+++ b/lessons_plan.xlsx
@@ -310,19 +310,19 @@
     <t>12-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação dos resultados do projeto intermediário</t>
+    <t xml:space="preserve">Entrega do projeto intermediário</t>
   </si>
   <si>
     <t>14-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação do status do projeto final</t>
+    <t xml:space="preserve">Desenvolvimento do projeto final</t>
   </si>
   <si>
     <t>19-Maio</t>
   </si>
   <si>
-    <t xml:space="preserve">Apresentação final do projeto</t>
+    <t xml:space="preserve">Entrega do projeto final</t>
   </si>
   <si>
     <t xml:space="preserve">Entrega da descrição dos métodos e resultados</t>
@@ -1117,7 +1117,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>